<commit_message>
feat: true dataset compression test
</commit_message>
<xml_diff>
--- a/data/string length.xlsx
+++ b/data/string length.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\protocolFish\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08EFEFA6-2F06-474B-AC75-163A3CFC72F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2066CB3A-3CC7-4B02-AD86-713331B54F9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17715" yWindow="4395" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2100" yWindow="3030" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>my</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -63,6 +64,21 @@
   <si>
     <t>my/json</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>step</t>
+  </si>
+  <si>
+    <t>my</t>
+  </si>
+  <si>
+    <t>protobuf</t>
+  </si>
+  <si>
+    <t>json</t>
+  </si>
+  <si>
+    <t>Process finished with exit code 0</t>
   </si>
 </sst>
 </file>
@@ -2894,7 +2910,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A91" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="D112" sqref="D112"/>
     </sheetView>
   </sheetViews>
@@ -6162,4 +6178,446 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F60309E5-AE1F-4F9B-92A3-91EF7140BD64}">
+  <dimension ref="A1:D32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>5</v>
+      </c>
+      <c r="B2">
+        <v>78618394</v>
+      </c>
+      <c r="C2">
+        <v>143080950</v>
+      </c>
+      <c r="D2">
+        <v>324611758</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>10</v>
+      </c>
+      <c r="B3">
+        <v>80710521</v>
+      </c>
+      <c r="C3">
+        <v>143080950</v>
+      </c>
+      <c r="D3">
+        <v>324611758</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>15</v>
+      </c>
+      <c r="B4">
+        <v>82491112</v>
+      </c>
+      <c r="C4">
+        <v>143080950</v>
+      </c>
+      <c r="D4">
+        <v>324611758</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>20</v>
+      </c>
+      <c r="B5">
+        <v>83839352</v>
+      </c>
+      <c r="C5">
+        <v>143080950</v>
+      </c>
+      <c r="D5">
+        <v>324611758</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>25</v>
+      </c>
+      <c r="B6">
+        <v>85375420</v>
+      </c>
+      <c r="C6">
+        <v>143080950</v>
+      </c>
+      <c r="D6">
+        <v>324611758</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>30</v>
+      </c>
+      <c r="B7">
+        <v>86617185</v>
+      </c>
+      <c r="C7">
+        <v>143080950</v>
+      </c>
+      <c r="D7">
+        <v>324611758</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>35</v>
+      </c>
+      <c r="B8">
+        <v>88006772</v>
+      </c>
+      <c r="C8">
+        <v>143080950</v>
+      </c>
+      <c r="D8">
+        <v>324611758</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>40</v>
+      </c>
+      <c r="B9">
+        <v>89105098</v>
+      </c>
+      <c r="C9">
+        <v>143080950</v>
+      </c>
+      <c r="D9">
+        <v>324611758</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>45</v>
+      </c>
+      <c r="B10">
+        <v>90438945</v>
+      </c>
+      <c r="C10">
+        <v>143080950</v>
+      </c>
+      <c r="D10">
+        <v>324611758</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>50</v>
+      </c>
+      <c r="B11">
+        <v>91517267</v>
+      </c>
+      <c r="C11">
+        <v>143080950</v>
+      </c>
+      <c r="D11">
+        <v>324611758</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>100</v>
+      </c>
+      <c r="B12">
+        <v>99054933</v>
+      </c>
+      <c r="C12">
+        <v>143080950</v>
+      </c>
+      <c r="D12">
+        <v>324611758</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>150</v>
+      </c>
+      <c r="B13">
+        <v>102067017</v>
+      </c>
+      <c r="C13">
+        <v>143080950</v>
+      </c>
+      <c r="D13">
+        <v>324611758</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>200</v>
+      </c>
+      <c r="B14">
+        <v>103920808</v>
+      </c>
+      <c r="C14">
+        <v>143080950</v>
+      </c>
+      <c r="D14">
+        <v>324611758</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>250</v>
+      </c>
+      <c r="B15">
+        <v>105124270</v>
+      </c>
+      <c r="C15">
+        <v>143080950</v>
+      </c>
+      <c r="D15">
+        <v>324611758</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>300</v>
+      </c>
+      <c r="B16">
+        <v>106015527</v>
+      </c>
+      <c r="C16">
+        <v>143080950</v>
+      </c>
+      <c r="D16">
+        <v>324611758</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>350</v>
+      </c>
+      <c r="B17">
+        <v>106757016</v>
+      </c>
+      <c r="C17">
+        <v>143080950</v>
+      </c>
+      <c r="D17">
+        <v>324611758</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>400</v>
+      </c>
+      <c r="B18">
+        <v>107342854</v>
+      </c>
+      <c r="C18">
+        <v>143080950</v>
+      </c>
+      <c r="D18">
+        <v>324611758</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>450</v>
+      </c>
+      <c r="B19">
+        <v>107808411</v>
+      </c>
+      <c r="C19">
+        <v>143080950</v>
+      </c>
+      <c r="D19">
+        <v>324611758</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>500</v>
+      </c>
+      <c r="B20">
+        <v>108211898</v>
+      </c>
+      <c r="C20">
+        <v>143080950</v>
+      </c>
+      <c r="D20">
+        <v>324611758</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>550</v>
+      </c>
+      <c r="B21">
+        <v>108539643</v>
+      </c>
+      <c r="C21">
+        <v>143080950</v>
+      </c>
+      <c r="D21">
+        <v>324611758</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>600</v>
+      </c>
+      <c r="B22">
+        <v>108854963</v>
+      </c>
+      <c r="C22">
+        <v>143080950</v>
+      </c>
+      <c r="D22">
+        <v>324611758</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>650</v>
+      </c>
+      <c r="B23">
+        <v>109255003</v>
+      </c>
+      <c r="C23">
+        <v>143080950</v>
+      </c>
+      <c r="D23">
+        <v>324611758</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>700</v>
+      </c>
+      <c r="B24">
+        <v>109378730</v>
+      </c>
+      <c r="C24">
+        <v>143080950</v>
+      </c>
+      <c r="D24">
+        <v>324611758</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>750</v>
+      </c>
+      <c r="B25">
+        <v>109831735</v>
+      </c>
+      <c r="C25">
+        <v>143080950</v>
+      </c>
+      <c r="D25">
+        <v>324611758</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>800</v>
+      </c>
+      <c r="B26">
+        <v>109892320</v>
+      </c>
+      <c r="C26">
+        <v>143080950</v>
+      </c>
+      <c r="D26">
+        <v>324611758</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>850</v>
+      </c>
+      <c r="B27">
+        <v>110158661</v>
+      </c>
+      <c r="C27">
+        <v>143080950</v>
+      </c>
+      <c r="D27">
+        <v>324611758</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>900</v>
+      </c>
+      <c r="B28">
+        <v>110191041</v>
+      </c>
+      <c r="C28">
+        <v>143080950</v>
+      </c>
+      <c r="D28">
+        <v>324611758</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>950</v>
+      </c>
+      <c r="B29">
+        <v>110203215</v>
+      </c>
+      <c r="C29">
+        <v>143080950</v>
+      </c>
+      <c r="D29">
+        <v>324611758</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>1000</v>
+      </c>
+      <c r="B30">
+        <v>110397692</v>
+      </c>
+      <c r="C30">
+        <v>143080950</v>
+      </c>
+      <c r="D30">
+        <v>324611758</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>